<commit_message>
exportacion de pdf y correcion de remision
</commit_message>
<xml_diff>
--- a/public/plantilla_excel.xlsx
+++ b/public/plantilla_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvarojapasalazar/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvarojapa/Desktop/cv alvaro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{309D74C6-2756-4541-82F7-345771146826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3121F3F3-A4E4-1445-8A19-D8FA16EBFFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{CA3DCBA9-FDC9-E546-AF02-B58117A627FF}"/>
+    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{4F72E8B0-60B7-A041-AA95-47372E1FBA04}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ITEM</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>FISCAL</t>
+  </si>
+  <si>
+    <t>PRECIO 4</t>
   </si>
 </sst>
 </file>
@@ -91,7 +94,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -110,13 +113,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,13 +134,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -153,26 +156,27 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -507,29 +511,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3406C5C7-6671-B64E-A0DB-769558E37606}">
-  <dimension ref="A1:P1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40F1E2F-A317-FE44-8F51-69CDFA689CD0}">
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P1"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -538,7 +542,7 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -554,17 +558,29 @@
         <v>11</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>